<commit_message>
making video resizeable :)
</commit_message>
<xml_diff>
--- a/dist/python/songs.xlsx
+++ b/dist/python/songs.xlsx
@@ -1062,7 +1062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -1096,1522 +1096,1654 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>2CELLOS - Shape Of My Heart [Live at Arena di Verona]</t>
+          <t>Kaleida - Think (Lyrics) John Wick soundtrack</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=jx1-NP9_YIA</t>
+          <t>https://www.youtube.com/watch?v=FVtFcbBfNYw</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Enrique Iglesias - EL BAÑO (Letra) ft. Bad Bunny</t>
+          <t>Hands Like Houses - Torn</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8BbtBnnnvCM</t>
+          <t>https://www.youtube.com/watch?v=M58IJO7N32s</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>2CELLOS - Love Story</t>
+          <t>E.Satie - Gnossienne N.1 (Piano)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=UdHopftQD3A</t>
+          <t>https://www.youtube.com/watch?v=X3JLOenXGUc</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lana Del Rey - Video Games</t>
+          <t>La Tormenta De Arena - Dorian (letra)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=cE6wxDqdOV0</t>
+          <t>https://www.youtube.com/watch?v=28W-KrHjmK8</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>2CELLOS - Fragile [LIVE at Arena Pula]</t>
+          <t>Yanni - Can't Wait (Sensuous Chill)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=q_ymIjOyzRQ</t>
+          <t>https://www.youtube.com/watch?v=9kardLhsFrk</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>Justin Bieber &amp; benny blanco - Lonely (Official Acoustic Video)</t>
+          <t>Zivert - Life (English Version)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Cu5hhxP_prE</t>
+          <t>https://www.youtube.com/watch?v=mTecGII7cFA</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>서태지와 아이들   이 밤이 깊어가지만 (가사 첨부)</t>
+          <t>Mariah Carey - My All [Lyrics]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=__SXVP2GmvM</t>
+          <t>https://www.youtube.com/watch?v=o4che1p-M4M</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cody Francis - Rose In The Garden</t>
+          <t>One Direction - Story of My Life</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=JO4-j1LfoQQ</t>
+          <t>https://www.youtube.com/watch?v=W-TE_Ys4iwM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>I Got Summer On My Mind (Still Dre Remix)</t>
+          <t>Beth Thornton - Something You Don't Know</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=89LOsf8pDhY</t>
+          <t>https://www.youtube.com/watch?v=RftohIbwlqg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lady Gaga, Bruno Mars - Die With A Smile</t>
+          <t>2CELLOS - Shape Of My Heart [Live at Arena di Verona]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=zgaCZOQCpp8</t>
+          <t>https://www.youtube.com/watch?v=jx1-NP9_YIA</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Maxim Fadeev - Googoosha</t>
+          <t>Enrique Iglesias - EL BAÑO (Letra) ft. Bad Bunny</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=gqOoJXttEec</t>
+          <t>https://www.youtube.com/watch?v=8BbtBnnnvCM</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>Elley Duhe - Middle Of The Night</t>
+          <t>2CELLOS - Love Story</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=KLTMCPzRO64</t>
+          <t>https://www.youtube.com/watch?v=UdHopftQD3A</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>Broken Angel (Albert Vishi ft. Taulant Sllamniku Cover)</t>
+          <t>Lana Del Rey - Video Games</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=5miHGQVFJm0</t>
+          <t>https://www.youtube.com/watch?v=cE6wxDqdOV0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>Laura Pausini - It’s Not Goodbye</t>
+          <t>2CELLOS - Fragile [LIVE at Arena Pula]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=onYQkI8S1UY</t>
+          <t>https://www.youtube.com/watch?v=q_ymIjOyzRQ</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Juice Wrld - Lucid Dreams </t>
+          <t>Justin Bieber &amp; benny blanco - Lonely (Official Acoustic Video)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=_fh64GbFSw4</t>
+          <t>https://www.youtube.com/watch?v=Cu5hhxP_prE</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ramz - Barking</t>
+          <t>서태지와 아이들   이 밤이 깊어가지만 (가사 첨부)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=Q0QKUU95bVc</t>
+          <t>https://www.youtube.com/watch?v=__SXVP2GmvM</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>falling in love with someone you can't have (a playlist)</t>
+          <t>Cody Francis - Rose In The Garden</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=_K57AlI62V4</t>
+          <t>https://www.youtube.com/watch?v=JO4-j1LfoQQ</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>Feeling Good 🌱 A playlist to lift your mood</t>
+          <t>I Got Summer On My Mind (Still Dre Remix)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=VYtBO_cDJCU</t>
+          <t>https://www.youtube.com/watch?v=89LOsf8pDhY</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>Best classical music: Beethoven, Mozart, Schubert,Bach...🎶</t>
+          <t>Lady Gaga, Bruno Mars - Die With A Smile</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=DxnDcH2NS5c</t>
+          <t>https://www.youtube.com/watch?v=zgaCZOQCpp8</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>Selena Gomez - Bad Liar</t>
+          <t>Maxim Fadeev - Googoosha</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NZKXkD6EgBk</t>
+          <t>https://www.youtube.com/watch?v=gqOoJXttEec</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>Florida Georgia Line - Simple (Lyrics)</t>
+          <t>Elley Duhe - Middle Of The Night</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TuTDc9d_9yI</t>
+          <t>https://www.youtube.com/watch?v=KLTMCPzRO64</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tones and I: Dance Monkey (US TV Debut)</t>
+          <t>Broken Angel (Albert Vishi ft. Taulant Sllamniku Cover)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=4iQxG8ZjYO8</t>
+          <t>https://www.youtube.com/watch?v=5miHGQVFJm0</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>the luka state - bring this all together</t>
+          <t>Laura Pausini - It’s Not Goodbye</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=OcJ5EgxsWBg</t>
+          <t>https://www.youtube.com/watch?v=onYQkI8S1UY</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sunset Sons - I Can`t Wait (Official Audio)</t>
+          <t xml:space="preserve">Juice Wrld - Lucid Dreams </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=JuiegvRQ8dI</t>
+          <t>https://www.youtube.com/watch?v=_fh64GbFSw4</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sunset Sons - Somewhere Maybe (Official Audio)</t>
+          <t>Ramz - Barking</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=SHapfmLyBp0</t>
+          <t>https://www.youtube.com/watch?v=Q0QKUU95bVc</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sunset Sons - Know My Name (Official Audio)</t>
+          <t>falling in love with someone you can't have (a playlist)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=orMwK0veDVQ</t>
+          <t>https://www.youtube.com/watch?v=_K57AlI62V4</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>Sunset Sons - The River</t>
+          <t>Feeling Good 🌱 A playlist to lift your mood</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=MCyEm1fViZQ</t>
+          <t>https://www.youtube.com/watch?v=VYtBO_cDJCU</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sunset Sons - Loa (Official Audio)</t>
+          <t>Best classical music: Beethoven, Mozart, Schubert,Bach...🎶</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9tXWQy7mMsM</t>
+          <t>https://www.youtube.com/watch?v=DxnDcH2NS5c</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sunset Song - On The Road (Lyrics)</t>
+          <t>Selena Gomez - Bad Liar</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=NsKZ-5EDqPA</t>
+          <t>https://www.youtube.com/watch?v=NZKXkD6EgBk</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sunset Sons - Remember</t>
+          <t>Florida Georgia Line - Simple (Lyrics)</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=PH_P12XqY9Y</t>
+          <t>https://www.youtube.com/watch?v=TuTDc9d_9yI</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>Craig David - Walking Away [Lyrics] 🎵</t>
+          <t>Tones and I: Dance Monkey (US TV Debut)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=8AwamgSDpdA</t>
+          <t>https://www.youtube.com/watch?v=4iQxG8ZjYO8</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>Escape (Rosaline OST)</t>
+          <t>the luka state - bring this all together</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=M9b_z-LKE14</t>
+          <t>https://www.youtube.com/watch?v=OcJ5EgxsWBg</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>Zara Larsson - Lush Life</t>
+          <t>Sunset Sons - I Can`t Wait (Official Audio)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=tD4HCZe-tew</t>
+          <t>https://www.youtube.com/watch?v=JuiegvRQ8dI</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>JEON SOMI DUMB DUMB Lyrics (전소미 DUMB DUMB 가사)</t>
+          <t>Sunset Sons - Somewhere Maybe (Official Audio)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TfAzTYzBvTo</t>
+          <t>https://www.youtube.com/watch?v=SHapfmLyBp0</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>Shakira - Can`t Remember to Forget You (Lyrics) ft. Rihanna</t>
+          <t>Sunset Sons - Know My Name (Official Audio)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=i_XM3u1_jZQ</t>
+          <t>https://www.youtube.com/watch?v=orMwK0veDVQ</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>Havana feat. Yaar &amp;amp; Kaiia - Last Night (Lyrics)</t>
+          <t>Sunset Sons - The River</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=i-Yuf5-zTec</t>
+          <t>https://www.youtube.com/watch?v=MCyEm1fViZQ</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>Craig David - Rise &amp; Fall ft. Sting (Official Video)</t>
+          <t>Sunset Sons - Loa (Official Audio)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=pU2ukeS2JTE</t>
+          <t>https://www.youtube.com/watch?v=9tXWQy7mMsM</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>Maroon 5 - Girls Like You ft. Cardi B (Official Music Video)</t>
+          <t>Sunset Song - On The Road (Lyrics)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=aJOTlE1K90k</t>
+          <t>https://www.youtube.com/watch?v=NsKZ-5EDqPA</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>Havana feat. Yaar &amp; Kaiia - Big Love (Official Video)</t>
+          <t>Sunset Sons - Remember</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=aVFNJBqj5vU</t>
+          <t>https://www.youtube.com/watch?v=PH_P12XqY9Y</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>Edward Maya, Vika Jigulina - Stereo love (Radio Edit) (Lyrics)</t>
+          <t>Craig David - Walking Away [Lyrics] 🎵</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=y9Kqb2z9Lzs</t>
+          <t>https://www.youtube.com/watch?v=8AwamgSDpdA</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>Gym Class Heroes: Stereo Hearts ft. Adam Levine</t>
+          <t>Escape (Rosaline OST)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=T3E9Wjbq44E</t>
+          <t>https://www.youtube.com/watch?v=M9b_z-LKE14</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>Shawn Mendes - It'll Be Okay</t>
+          <t>Zara Larsson - Lush Life</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://youtu.be/KrgJp7Z1Hv8?si=MOyY5rZzP-7kcfhM</t>
+          <t>https://www.youtube.com/watch?v=tD4HCZe-tew</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>somewhere only we know (Gustixa &amp;amp; Rhianne)</t>
+          <t>JEON SOMI DUMB DUMB Lyrics (전소미 DUMB DUMB 가사)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=92izkAK5OA0</t>
+          <t>https://www.youtube.com/watch?v=TfAzTYzBvTo</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>Duncan Laurence feat. FLETCHER – Arcade</t>
+          <t>Shakira - Can`t Remember to Forget You (Lyrics) ft. Rihanna</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=308v08mFWWc</t>
+          <t>https://www.youtube.com/watch?v=i_XM3u1_jZQ</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>Bad Liar (cover)</t>
+          <t>Havana feat. Yaar &amp;amp; Kaiia - Last Night (Lyrics)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://youtu.be/5jfz3q9Z0RY?si=OHvyb7AMtM_wtAXc</t>
+          <t>https://www.youtube.com/watch?v=i-Yuf5-zTec</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>Lana Del Rey - Summertime Sadness (Official Music Video)</t>
+          <t>Craig David - Rise &amp; Fall ft. Sting (Official Video)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=TdrL3QxjyVw</t>
+          <t>https://www.youtube.com/watch?v=pU2ukeS2JTE</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>Linkin Park - In The End (Mellen Gi &amp;amp; Tommee Profitt Remix)</t>
+          <t>Maroon 5 - Girls Like You ft. Cardi B (Official Music Video)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=WNeLUngb-Xg</t>
+          <t>https://www.youtube.com/watch?v=aJOTlE1K90k</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
         <is>
-          <t>Enya - Only Time (Official 4K Music Video)</t>
+          <t>Havana feat. Yaar &amp; Kaiia - Big Love (Official Video)</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=7wfYIMyS_dI</t>
+          <t>https://www.youtube.com/watch?v=aVFNJBqj5vU</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>Today is a Good Day</t>
+          <t>Edward Maya, Vika Jigulina - Stereo love (Radio Edit) (Lyrics)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://youtu.be/9L4EjJqrz0c?si=x97RAvAA9IELRZPW</t>
+          <t>https://www.youtube.com/watch?v=y9Kqb2z9Lzs</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
         <is>
-          <t>Heroes Tonight</t>
+          <t>Gym Class Heroes: Stereo Hearts ft. Adam Levine</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=074rfF4RJZc</t>
+          <t>https://www.youtube.com/watch?v=T3E9Wjbq44E</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
         <is>
-          <t>Shakira - Hips Dont Lie</t>
+          <t>Shawn Mendes - It'll Be Okay</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://youtu.be/p3pEe6aAJ4k?si=bzrAEs7c-zSwqBUo</t>
+          <t>https://youtu.be/KrgJp7Z1Hv8?si=MOyY5rZzP-7kcfhM</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
         <is>
-          <t>Shakira - La La La World Cup 2014</t>
+          <t>somewhere only we know (Gustixa &amp;amp; Rhianne)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://youtu.be/2igups6VdcA?si=N5uu5genirJuWXWC</t>
+          <t>https://www.youtube.com/watch?v=92izkAK5OA0</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="inlineStr">
         <is>
-          <t>Something Just Like This</t>
+          <t>Duncan Laurence feat. FLETCHER – Arcade</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://youtu.be/FM7MFYoylVs?si=TrbAGj-JAUeEJ4bd</t>
+          <t>https://www.youtube.com/watch?v=308v08mFWWc</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="inlineStr">
         <is>
-          <t>Shakira - Chantaje (letra)</t>
+          <t>Bad Liar (cover)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://youtu.be/J76eQJP3UIQ?si=juYKqG_UCEta8y19</t>
+          <t>https://youtu.be/5jfz3q9Z0RY?si=OHvyb7AMtM_wtAXc</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="inlineStr">
         <is>
-          <t>Zara Larsson – Dont Worry Bout Me</t>
+          <t>Lana Del Rey - Summertime Sadness (Official Music Video)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://youtu.be/u_tzZd9kIWg?si=y-s2yCVh4U2JLsJJ</t>
+          <t>https://www.youtube.com/watch?v=TdrL3QxjyVw</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="inlineStr">
         <is>
-          <t>Selena Gomez - Buscando Amor</t>
+          <t>Linkin Park - In The End (Mellen Gi &amp;amp; Tommee Profitt Remix)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://youtu.be/2P6EExu3H5s?si=f2hv9y52VqxnVOmL</t>
+          <t>https://www.youtube.com/watch?v=WNeLUngb-Xg</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>Shawn Mendes - In My Blood</t>
+          <t>Enya - Only Time (Official 4K Music Video)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://youtu.be/36tggrpRoTI?si=CiCfVdO8Oepjt4Rs</t>
+          <t>https://www.youtube.com/watch?v=7wfYIMyS_dI</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>Charlie Puth - We Dont Talk Anymore</t>
+          <t>Today is a Good Day</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://youtu.be/bpFVJJBgtXY?si=L2NuwOWGhmdKacwg</t>
+          <t>https://youtu.be/9L4EjJqrz0c?si=x97RAvAA9IELRZPW</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>Selena Gomez - Adiós</t>
+          <t>Heroes Tonight</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://youtu.be/9H_368c2Hzw?si=UOBGyTGbUe_fISFW</t>
+          <t>https://www.youtube.com/watch?v=074rfF4RJZc</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>Charlie Puth - Attention</t>
+          <t>Shakira - Hips Dont Lie</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://youtu.be/Oz5JDtkf1as</t>
+          <t>https://youtu.be/p3pEe6aAJ4k?si=bzrAEs7c-zSwqBUo</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="inlineStr">
         <is>
-          <t>Bruno Mars - Grenade</t>
+          <t>Shakira - La La La World Cup 2014</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://youtu.be/4YrzJ9RZ9qY</t>
+          <t>https://youtu.be/2igups6VdcA?si=N5uu5genirJuWXWC</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>Let Me Love You</t>
+          <t>Something Just Like This</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://youtu.be/SMs0GnYze34?si=T-UORWGqJCoitcOM</t>
+          <t>https://youtu.be/FM7MFYoylVs?si=TrbAGj-JAUeEJ4bd</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>Sweet But Psycho</t>
+          <t>Shakira - Chantaje (letra)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://youtu.be/2KBFD0aoZy8</t>
+          <t>https://youtu.be/J76eQJP3UIQ?si=juYKqG_UCEta8y19</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>Who`s laughing now - Ava Max</t>
+          <t>Zara Larsson – Dont Worry Bout Me</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://youtu.be/4JYSgIiSZSA?si=3v9kDuzvYJvWaOsO</t>
+          <t>https://youtu.be/u_tzZd9kIWg?si=y-s2yCVh4U2JLsJJ</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="inlineStr">
         <is>
-          <t>Girls Like You</t>
+          <t>Selena Gomez - Buscando Amor</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://youtu.be/aJOTlE1K90k</t>
+          <t>https://youtu.be/2P6EExu3H5s?si=f2hv9y52VqxnVOmL</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="inlineStr">
         <is>
-          <t>Camila Cabello - Havana</t>
+          <t>Shawn Mendes - In My Blood</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://youtu.be/HCjNJDNzw8Y?si=QjZAi7GPIc4ParOQ</t>
+          <t>https://youtu.be/36tggrpRoTI?si=CiCfVdO8Oepjt4Rs</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="inlineStr">
         <is>
-          <t>Maroon 5 - Memories</t>
+          <t>Charlie Puth - We Dont Talk Anymore</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=SlPhMPnQ58k&amp;pp=ygUPbWFyb29uIG1lbW9yaWVz</t>
+          <t>https://youtu.be/bpFVJJBgtXY?si=L2NuwOWGhmdKacwg</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>post malone - rockstar (feat. 21 savage)</t>
+          <t>Selena Gomez - Adiós</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9lQP9-F8kIQ</t>
+          <t>https://youtu.be/9H_368c2Hzw?si=UOBGyTGbUe_fISFW</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="inlineStr">
         <is>
-          <t>Drake - Gods plan</t>
+          <t>Charlie Puth - Attention</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=ScfgOVJiu_I</t>
+          <t>https://youtu.be/Oz5JDtkf1as</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>Dua Lipa - Levitating</t>
+          <t>Bruno Mars - Grenade</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=j2c3tR_qfiQ</t>
+          <t>https://youtu.be/4YrzJ9RZ9qY</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>Justin Bieber - Baby</t>
+          <t>Let Me Love You</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=khOFw2f4bQY</t>
+          <t>https://youtu.be/SMs0GnYze34?si=T-UORWGqJCoitcOM</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>State of Grace</t>
+          <t>Sweet But Psycho</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=gr4cqcqnAN0</t>
+          <t>https://youtu.be/2KBFD0aoZy8</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>Taylor Swift - Back To December</t>
+          <t>Who`s laughing now - Ava Max</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://youtu.be/QUwxKWT6m7U?si=LNPBWKl0DqXIfOP2</t>
+          <t>https://youtu.be/4JYSgIiSZSA?si=3v9kDuzvYJvWaOsO</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>As it was</t>
+          <t>Girls Like You</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://youtu.be/Qfm6nfz1QNQ?si=3mMjYFpALij7GELl</t>
+          <t>https://youtu.be/aJOTlE1K90k</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>Taylor Swift - Begin Again</t>
+          <t>Camila Cabello - Havana</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://youtu.be/cMPEd8m79Hw?si=9zE5-51p0xGyEgSO</t>
+          <t>https://youtu.be/HCjNJDNzw8Y?si=QjZAi7GPIc4ParOQ</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
-          <t>Sofia</t>
+          <t>Maroon 5 - Memories</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://youtu.be/ftI_Lp7LAuU?si=aOFT5Ral2-A_2PxG</t>
+          <t>https://www.youtube.com/watch?v=SlPhMPnQ58k&amp;pp=ygUPbWFyb29uIG1lbW9yaWVz</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>Numb (lyrics|rock)</t>
+          <t>post malone - rockstar (feat. 21 savage)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://youtu.be/8P0vKLHbtMg?si=HhXMHjE8vD2yeC_B</t>
+          <t>https://www.youtube.com/watch?v=9lQP9-F8kIQ</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="inlineStr">
         <is>
-          <t>For The Rest Of My Life</t>
+          <t>Drake - Gods plan</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://youtu.be/PHbZ9SXHJwA?si=_7a2Gaka2oPEWrCQ</t>
+          <t>https://www.youtube.com/watch?v=ScfgOVJiu_I</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
-          <t>Insha Allah</t>
+          <t>Dua Lipa - Levitating</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://youtu.be/8xXJyFNfiy8?si=XkqgGm4hEyZoqJe1</t>
+          <t>https://www.youtube.com/watch?v=j2c3tR_qfiQ</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>Hunger Games | Atlas</t>
+          <t>Justin Bieber - Baby</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://youtu.be/Lh3TokLzzmw?si=I5CcdBNIEuwDZvVT</t>
+          <t>https://www.youtube.com/watch?v=khOFw2f4bQY</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="inlineStr">
         <is>
-          <t>Hard To Say Im Sorry</t>
+          <t>State of Grace</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://youtu.be/XCmOdVia9DE?si=60M6i15UUakuL7DH</t>
+          <t>https://www.youtube.com/watch?v=gr4cqcqnAN0</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
         <is>
-          <t>Sasha Sloan - Lie</t>
+          <t>Taylor Swift - Back To December</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://youtu.be/AzjTJpzfB8U?si=PHYxAGETm1P1opd0</t>
+          <t>https://youtu.be/QUwxKWT6m7U?si=LNPBWKl0DqXIfOP2</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
-          <t>Solo Para Ti</t>
+          <t>As it was</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://youtu.be/5D_A4IBWSv4?si=pgNinSqUyLBks6po</t>
+          <t>https://youtu.be/Qfm6nfz1QNQ?si=3mMjYFpALij7GELl</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="inlineStr">
         <is>
-          <t>Zara Larsson - This Ones For You</t>
+          <t>Taylor Swift - Begin Again</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>https://youtu.be/MoHnffhBwqs?si=_FGX4ucMtOTcD2to</t>
+          <t>https://youtu.be/cMPEd8m79Hw?si=9zE5-51p0xGyEgSO</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="inlineStr">
         <is>
-          <t>La Cintura</t>
+          <t>Sofia</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>https://youtu.be/Eg4LUvUjUWI?si=YqeuNfTh_iTuj-dP</t>
+          <t>https://youtu.be/ftI_Lp7LAuU?si=aOFT5Ral2-A_2PxG</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>Diamond Heart</t>
+          <t>Numb (lyrics|rock)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>https://youtu.be/bcHoBDw4G10?si=auASu-G_c9NkS48Z</t>
+          <t>https://youtu.be/8P0vKLHbtMg?si=HhXMHjE8vD2yeC_B</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>Halsey - Sorry</t>
+          <t>For The Rest Of My Life</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>https://youtu.be/CPAoMCo7tNw?si=2rEiXXCn6UcySUVZ</t>
+          <t>https://youtu.be/PHbZ9SXHJwA?si=_7a2Gaka2oPEWrCQ</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>Relax, Take it Easy</t>
+          <t>Insha Allah</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>https://youtu.be/EVDYmBrl02Q?si=ODB07HFZCtTtg4F4</t>
+          <t>https://youtu.be/8xXJyFNfiy8?si=XkqgGm4hEyZoqJe1</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="inlineStr">
         <is>
-          <t>Thank you Allah</t>
+          <t>Hunger Games | Atlas</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>https://youtu.be/RBrdl0v_anc?si=cu3qNsVyUIIzZGvv</t>
+          <t>https://youtu.be/Lh3TokLzzmw?si=I5CcdBNIEuwDZvVT</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>Let me down slowly</t>
+          <t>Hard To Say Im Sorry</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>https://youtu.be/50VNCymT-Cs?si=sEwBTlJCeuqL9LTD</t>
+          <t>https://youtu.be/XCmOdVia9DE?si=60M6i15UUakuL7DH</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="inlineStr">
         <is>
-          <t>Lonely (acoustic)</t>
+          <t>Sasha Sloan - Lie</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>https://youtu.be/Cu5hhxP_prE?si=VRZVlVcLWqk8Dasg</t>
+          <t>https://youtu.be/AzjTJpzfB8U?si=PHYxAGETm1P1opd0</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>Selfish love</t>
+          <t>Solo Para Ti</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>https://youtu.be/9gqAq6kq5Ek?si=Gro32XWDuPLWzyIv</t>
+          <t>https://youtu.be/5D_A4IBWSv4?si=pgNinSqUyLBks6po</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>twenty one pilots: Heathens</t>
+          <t>Zara Larsson - This Ones For You</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>https://youtu.be/UprcpdwuwCg?si=O6_fwxx8TOkfjIXi</t>
+          <t>https://youtu.be/MoHnffhBwqs?si=_FGX4ucMtOTcD2to</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>Dont Let Me Down</t>
+          <t>La Cintura</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>https://youtu.be/Io0fBr1XBUA?si=SUp9MdCXlOU_Vf5s</t>
+          <t>https://youtu.be/Eg4LUvUjUWI?si=YqeuNfTh_iTuj-dP</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>Someone you loved</t>
+          <t>Diamond Heart</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>https://youtu.be/zABLecsR5UE?si=k3rryaA0P3O8JBhY</t>
+          <t>https://youtu.be/bcHoBDw4G10?si=auASu-G_c9NkS48Z</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="inlineStr">
         <is>
-          <t>Fed up with us</t>
+          <t>Halsey - Sorry</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>https://youtu.be/n1NTv6Y4pxs?si=76WA3JI0TGILBHm7</t>
+          <t>https://youtu.be/CPAoMCo7tNw?si=2rEiXXCn6UcySUVZ</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>Skyfall</t>
+          <t>Relax, Take it Easy</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>https://youtu.be/DeumyOzKqgI?si=Cok0dR7byK6pN682</t>
+          <t>https://youtu.be/EVDYmBrl02Q?si=ODB07HFZCtTtg4F4</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="inlineStr">
         <is>
-          <t>Story of my life</t>
+          <t>Thank you Allah</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>https://youtu.be/W-TE_Ys4iwM?si=RViOxRuaXxdz3pmm</t>
+          <t>https://youtu.be/RBrdl0v_anc?si=cu3qNsVyUIIzZGvv</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="inlineStr">
         <is>
-          <t>Reamonn - Tonight</t>
+          <t>Let me down slowly</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>https://youtu.be/jtoncUzV6nA?si=yULSO1-MxnAVV13i</t>
+          <t>https://youtu.be/50VNCymT-Cs?si=sEwBTlJCeuqL9LTD</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="inlineStr">
         <is>
-          <t>Hymn For The Weekend</t>
+          <t>Lonely (acoustic)</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=YykjpeuMNEk</t>
+          <t>https://youtu.be/Cu5hhxP_prE?si=VRZVlVcLWqk8Dasg</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="inlineStr">
         <is>
-          <t>Hell Or High Water</t>
+          <t>Selfish love</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>https://youtu.be/zgDbp5C74sU?si=R8Q5HZq2vzhGL57g</t>
+          <t>https://youtu.be/9gqAq6kq5Ek?si=Gro32XWDuPLWzyIv</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="inlineStr">
         <is>
-          <t>Everything I Need</t>
+          <t>twenty one pilots: Heathens</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9bCp7j3nC30</t>
+          <t>https://youtu.be/UprcpdwuwCg?si=O6_fwxx8TOkfjIXi</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="inlineStr">
         <is>
-          <t>Love the way you lie</t>
+          <t>Dont Let Me Down</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>https://youtu.be/h_-JFUci0BM?si=SHiuHs1NdIjpN0WP</t>
+          <t>https://youtu.be/Io0fBr1XBUA?si=SUp9MdCXlOU_Vf5s</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="inlineStr">
         <is>
-          <t>Moving Mountains</t>
+          <t>Someone you loved</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>https://youtu.be/S_0r3hYg78o?si=Be6GShy7mgRcl9Ha</t>
+          <t>https://youtu.be/zABLecsR5UE?si=k3rryaA0P3O8JBhY</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="inlineStr">
         <is>
-          <t>Numb (cover)</t>
+          <t>Fed up with us</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>https://youtu.be/gHp-OjLOG5A?si=0abUDswbKz6rhQeX</t>
+          <t>https://youtu.be/n1NTv6Y4pxs?si=76WA3JI0TGILBHm7</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="inlineStr">
         <is>
-          <t>Until I found you</t>
+          <t>Skyfall</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>https://youtu.be/oIKuyj2GQtY</t>
+          <t>https://youtu.be/DeumyOzKqgI?si=Cok0dR7byK6pN682</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="inlineStr">
         <is>
-          <t>Heart is on fire</t>
+          <t>Story of my life</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>https://youtu.be/kBqqlW6-99M?si=kXaaJTqhA4PaY6Gd</t>
+          <t>https://youtu.be/W-TE_Ys4iwM?si=RViOxRuaXxdz3pmm</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="inlineStr">
         <is>
-          <t>Holes</t>
+          <t>Reamonn - Tonight</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>https://youtu.be/DeFWClW7skQ?si=hkIGl-CTTw-FbnLz</t>
+          <t>https://youtu.be/jtoncUzV6nA?si=yULSO1-MxnAVV13i</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="inlineStr">
         <is>
-          <t>Survivors</t>
+          <t>Hymn For The Weekend</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=vN0gaXS8dQE</t>
+          <t>https://www.youtube.com/watch?v=YykjpeuMNEk</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="B111" t="inlineStr">
         <is>
-          <t>Irakliy - Ya s toboy(cover)</t>
+          <t>Hell Or High Water</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>https://youtu.be/3WmdZOF5bKk?si=LcXY8Gohxxx4cZSA</t>
+          <t>https://youtu.be/zgDbp5C74sU?si=R8Q5HZq2vzhGL57g</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="inlineStr">
         <is>
-          <t>Vetrom stat (cover)</t>
+          <t>Everything I Need</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>https://youtu.be/kkzEs0gdvZI?si=Z456wgKuJd0aE_PA</t>
+          <t>https://www.youtube.com/watch?v=9bCp7j3nC30</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="inlineStr">
         <is>
-          <t>Reamonn - Supergirl</t>
+          <t>Love the way you lie</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>https://youtu.be/ctmS5XX67Ek?si=NGZGPw0bcpfZciyi</t>
+          <t>https://youtu.be/h_-JFUci0BM?si=SHiuHs1NdIjpN0WP</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="inlineStr">
         <is>
-          <t>Another Love</t>
+          <t>Moving Mountains</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>https://youtu.be/Jkj36B1YuDU?si=Yku5tRPe7avRNr2R</t>
+          <t>https://youtu.be/S_0r3hYg78o?si=Be6GShy7mgRcl9Ha</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="B115" t="inlineStr">
         <is>
-          <t>All the little lights</t>
+          <t>Numb (cover)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>https://youtu.be/OkxVxox--Io?si=AE4wj_c_uqTWGrbB</t>
+          <t>https://youtu.be/gHp-OjLOG5A?si=0abUDswbKz6rhQeX</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="inlineStr">
         <is>
-          <t>Arcade</t>
+          <t>Until I found you</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>https://youtu.be/Qau6mObfSGM?si=RsrcZ0VUCOHaEwE4</t>
+          <t>https://youtu.be/oIKuyj2GQtY</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="B117" t="inlineStr">
         <is>
-          <t>Burito - Po volnam</t>
+          <t>Heart is on fire</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>https://youtu.be/jqyJ4xW2gb0?si=VgrA4JKMWkeWDIA5</t>
+          <t>https://youtu.be/kBqqlW6-99M?si=kXaaJTqhA4PaY6Gd</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="inlineStr">
         <is>
-          <t>To Be Free</t>
+          <t>Holes</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>https://youtu.be/hNd5pILkpSw?si=qiwZxiuS0yeiuOPs</t>
+          <t>https://youtu.be/DeFWClW7skQ?si=hkIGl-CTTw-FbnLz</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="B119" t="inlineStr">
         <is>
-          <t>Castle of Glass</t>
+          <t>Survivors</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=PPkJeWPP2nM</t>
+          <t>https://www.youtube.com/watch?v=vN0gaXS8dQE</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="B120" t="inlineStr">
         <is>
-          <t>Ava Max - Alone</t>
+          <t>Irakliy - Ya s toboy(cover)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>https://youtu.be/omvW1cI-3xg?si=zHiFadZaUUpddcgu</t>
+          <t>https://youtu.be/3WmdZOF5bKk?si=LcXY8Gohxxx4cZSA</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="B121" t="inlineStr">
         <is>
-          <t>Let Her Go (ft Ed Sheeran)</t>
+          <t>Vetrom stat (cover)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>https://youtu.be/HTcL9WkB_wg?si=ILXw9EaPM4GJyx29</t>
+          <t>https://youtu.be/kkzEs0gdvZI?si=Z456wgKuJd0aE_PA</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="inlineStr">
         <is>
-          <t>In the end (rmx)</t>
+          <t>Reamonn - Supergirl</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>https://youtu.be/WNeLUngb-Xg?si=V95nGOt0sMvhQG7c</t>
+          <t>https://youtu.be/ctmS5XX67Ek?si=NGZGPw0bcpfZciyi</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="B123" t="inlineStr">
         <is>
-          <t>No Time To Die</t>
+          <t>Another Love</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>https://youtu.be/GB_S2qFh5lU?si=XDH6CdXhqJq-g321</t>
+          <t>https://youtu.be/Jkj36B1YuDU?si=Yku5tRPe7avRNr2R</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="inlineStr">
         <is>
-          <t>The Cup Of Life - Ricky Martin</t>
+          <t>All the little lights</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>https://youtu.be/CBfSeqfeggI?si=A2RRcM0PSvAsvpHF</t>
+          <t>https://youtu.be/OkxVxox--Io?si=AE4wj_c_uqTWGrbB</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="inlineStr">
         <is>
-          <t>Баста - Выпускной</t>
+          <t>Arcade</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>https://youtu.be/t1-yL-xvklc?si=YZ1rS5hZtleOFOy1</t>
+          <t>https://youtu.be/Qau6mObfSGM?si=RsrcZ0VUCOHaEwE4</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="inlineStr">
         <is>
-          <t>Wonderful Life</t>
+          <t>Burito - Po volnam</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>https://youtu.be/qzn_6bXdgeE?si=BgnimyD5Frnn_-o-</t>
+          <t>https://youtu.be/jqyJ4xW2gb0?si=VgrA4JKMWkeWDIA5</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="B127" t="inlineStr">
         <is>
-          <t>Shape of My Heart</t>
+          <t>To Be Free</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>https://youtu.be/pm3rDbXbZRI?si=7TxDuViBxhHGeZoU</t>
+          <t>https://youtu.be/hNd5pILkpSw?si=qiwZxiuS0yeiuOPs</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="inlineStr">
         <is>
+          <t>Castle of Glass</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=PPkJeWPP2nM</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Ava Max - Alone</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://youtu.be/omvW1cI-3xg?si=zHiFadZaUUpddcgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Let Her Go (ft Ed Sheeran)</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>https://youtu.be/HTcL9WkB_wg?si=ILXw9EaPM4GJyx29</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>In the end (rmx)</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://youtu.be/WNeLUngb-Xg?si=V95nGOt0sMvhQG7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>No Time To Die</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://youtu.be/GB_S2qFh5lU?si=XDH6CdXhqJq-g321</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>The Cup Of Life - Ricky Martin</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://youtu.be/CBfSeqfeggI?si=A2RRcM0PSvAsvpHF</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Баста - Выпускной</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://youtu.be/t1-yL-xvklc?si=YZ1rS5hZtleOFOy1</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Wonderful Life</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://youtu.be/qzn_6bXdgeE?si=BgnimyD5Frnn_-o-</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Shape of My Heart</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://youtu.be/pm3rDbXbZRI?si=7TxDuViBxhHGeZoU</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Wonderful Life</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://youtu.be/qzn_6bXdgeE?si=BgnimyD5Frnn_-o-</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Shape of My Heart</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://youtu.be/pm3rDbXbZRI?si=7TxDuViBxhHGeZoU</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="inlineStr">
+        <is>
           <t>Tired Of Being Sorry</t>
         </is>
       </c>
-      <c r="C128" t="inlineStr">
+      <c r="C139" t="inlineStr">
         <is>
           <t>https://youtu.be/gzFmctgW0s8?si=JfvG_0Sj-IdPWoBY</t>
         </is>

</xml_diff>